<commit_message>
Agenda now has weapons/Eula Support
</commit_message>
<xml_diff>
--- a/GenshinCharacters.xlsx
+++ b/GenshinCharacters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gtoad\Documents\BlobBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D4B5DB-1B90-42E4-BD1E-459768B7642F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2AE5A0-3EB8-4461-86ED-13187515B29A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF13A9D8-420D-40BB-A6AF-029FCE87685E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{DF13A9D8-420D-40BB-A6AF-029FCE87685E}"/>
   </bookViews>
   <sheets>
     <sheet name="GenshinCharacters" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="122">
   <si>
     <t>Amber</t>
   </si>
@@ -390,6 +390,15 @@
   </si>
   <si>
     <t>Jueyun Chili</t>
+  </si>
+  <si>
+    <t>Eula</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/a5RHtCI.jpg</t>
+  </si>
+  <si>
+    <t>Crystalline Bloom</t>
   </si>
 </sst>
 </file>
@@ -458,7 +467,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -471,6 +480,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,10 +719,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F47B9A25-0A8F-46A2-BC59-42177149DADA}" name="Table1" displayName="Table1" ref="A1:I33" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I33" xr:uid="{1B40953C-B0B8-4969-BB81-BB1F0E953D27}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D33">
-    <sortCondition ref="A1:A33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F47B9A25-0A8F-46A2-BC59-42177149DADA}" name="Table1" displayName="Table1" ref="A1:I34" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I34" xr:uid="{1B40953C-B0B8-4969-BB81-BB1F0E953D27}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I34">
+    <sortCondition ref="A1:A34"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8969A4DD-9AD9-4EFD-A0CE-120AB9A5D068}" name="Character" totalsRowLabel="Total" dataDxfId="8"/>
@@ -1030,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F93B45E4-1E46-4A4C-B55A-236C3809F130}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1090,7 +1100,7 @@
         <v>38</v>
       </c>
       <c r="D2" s="1" t="str">
-        <f t="shared" ref="D2:D25" si="0">IF($C2="Freedom","Monday, Thursday, Sunday",IF($C2="Ballad","Wednesday, Saturday, Sunday",IF($C2="Resistance","Tuesday, Friday, Sunday",IF($C2="Prosperity","Monday, Thursday, Sunday",IF($C2="Diligence","Tuesday, Friday, Sunday",IF($C2="Gold","Wednesday, Saturday, Sunday"))))))</f>
+        <f t="shared" ref="D2:D26" si="0">IF($C2="Freedom","Monday, Thursday, Sunday",IF($C2="Ballad","Wednesday, Saturday, Sunday",IF($C2="Resistance","Tuesday, Friday, Sunday",IF($C2="Prosperity","Monday, Thursday, Sunday",IF($C2="Diligence","Tuesday, Friday, Sunday",IF($C2="Gold","Wednesday, Saturday, Sunday"))))))</f>
         <v>Wednesday, Saturday, Sunday</v>
       </c>
       <c r="E2" s="7" t="s">
@@ -1100,7 +1110,7 @@
         <v>89</v>
       </c>
       <c r="G2" s="1" t="str">
-        <f t="shared" ref="G2:G33" si="1">IF($B2="Geo","Prithiva Topaz (Geo Hypostasis)",IF($B2="Pyro","Agnidus Agate (Pyro Regisvine)",IF($B2="Hydro","Varunada Lazurite (Oceanid)",IF($B2="Electro","Vajrada Amethyst (Electro Hypostasis)",IF($B2="Cryo","Shivada Jade (Cryo Regisvine)",IF($B2="Anemo","Vayuda Turquoise (Anemo Hypostasis)"))))))</f>
+        <f t="shared" ref="G2:G26" si="1">IF($B2="Geo","Prithiva Topaz (Geo Hypostasis)",IF($B2="Pyro","Agnidus Agate (Pyro Regisvine)",IF($B2="Hydro","Varunada Lazurite (Oceanid)",IF($B2="Electro","Vajrada Amethyst (Electro Hypostasis)",IF($B2="Cryo","Shivada Jade (Cryo Regisvine)",IF($B2="Anemo","Vayuda Turquoise (Anemo Hypostasis)"))))))</f>
         <v>Prithiva Topaz (Geo Hypostasis)</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1328,73 +1338,73 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
+      <c r="A10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Wednesday, Saturday, Sunday</v>
+        <v>Tuesday, Friday, Sunday</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="G10" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Vajrada Amethyst (Electro Hypostasis)</v>
+        <v>120</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Shivada Jade (Cryo Regisvine)</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Wednesday, Saturday, Sunday</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Vajrada Amethyst (Electro Hypostasis)</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Tuesday, Friday, Sunday</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Shivada Jade (Cryo Regisvine)</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>40</v>
@@ -1403,256 +1413,256 @@
         <f t="shared" si="0"/>
         <v>Tuesday, Friday, Sunday</v>
       </c>
-      <c r="E12" s="7" t="s">
-        <v>67</v>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Agnidus Agate (Pyro Regisvine)</v>
+        <v>Shivada Jade (Cryo Regisvine)</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>32</v>
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday, Friday, Sunday</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>68</v>
+      <c r="E13" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
+        <v>Agnidus Agate (Pyro Regisvine)</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Wednesday, Saturday, Sunday</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>69</v>
+        <v>Tuesday, Friday, Sunday</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="G14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Shivada Jade (Cryo Regisvine)</v>
+        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Monday, Thursday, Sunday</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>70</v>
+        <v>Wednesday, Saturday, Sunday</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Vajrada Amethyst (Electro Hypostasis)</v>
+        <v>Shivada Jade (Cryo Regisvine)</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Monday, Thursday, Sunday</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Agnidus Agate (Pyro Regisvine)</v>
+        <v>Vajrada Amethyst (Electro Hypostasis)</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Wednesday, Saturday, Sunday</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>72</v>
+        <v>Monday, Thursday, Sunday</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Vajrada Amethyst (Electro Hypostasis)</v>
+        <v>Agnidus Agate (Pyro Regisvine)</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Tuesday, Friday, Sunday</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>Wednesday, Saturday, Sunday</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Varunada Lazurite (Oceanid)</v>
+        <v>Vajrada Amethyst (Electro Hypostasis)</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Monday, Thursday, Sunday</v>
+        <v>Tuesday, Friday, Sunday</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Prithiva Topaz (Geo Hypostasis)</v>
+        <v>Varunada Lazurite (Oceanid)</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Tuesday, Friday, Sunday</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>75</v>
+        <v>Monday, Thursday, Sunday</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>89</v>
@@ -1662,142 +1672,142 @@
         <v>Prithiva Topaz (Geo Hypostasis)</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>Monday, Thursday, Sunday</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>76</v>
+        <v>Tuesday, Friday, Sunday</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Shivada Jade (Cryo Regisvine)</v>
+        <v>Prithiva Topaz (Geo Hypostasis)</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Monday, Thursday, Sunday</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Shivada Jade (Cryo Regisvine)</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="1" t="str">
+      <c r="D23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Tuesday, Friday, Sunday</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="G22" s="1" t="str">
+      <c r="G23" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Vajrada Amethyst (Electro Hypostasis)</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="H23" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B24" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="1" t="str">
+      <c r="D24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Wednesday, Saturday, Sunday</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G23" s="1" t="str">
+      <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Shivada Jade (Cryo Regisvine)</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H24" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="I24" s="1" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f t="shared" si="0"/>
-        <v>Monday, Thursday, Sunday</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G24" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>37</v>
@@ -1807,181 +1817,181 @@
         <v>Monday, Thursday, Sunday</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>Varunada Lazurite (Oceanid)</v>
+        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>56</v>
+        <v>37</v>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Monday, Thursday, Sunday</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>54</v>
+        <v>94</v>
+      </c>
+      <c r="G26" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>Varunada Lazurite (Oceanid)</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f t="shared" ref="D27:D33" si="2">IF($C27="Freedom","Monday, Thursday, Sunday",IF($C27="Ballad","Wednesday, Saturday, Sunday",IF($C27="Resistance","Tuesday, Friday, Sunday",IF($C27="Prosperity","Monday, Thursday, Sunday",IF($C27="Diligence","Tuesday, Friday, Sunday",IF($C27="Gold","Wednesday, Saturday, Sunday"))))))</f>
-        <v>Wednesday, Saturday, Sunday</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>81</v>
+        <v>41</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>56</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G27" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
+        <v>117</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="str">
+        <f t="shared" ref="D28:D34" si="2">IF($C28="Freedom","Monday, Thursday, Sunday",IF($C28="Ballad","Wednesday, Saturday, Sunday",IF($C28="Resistance","Tuesday, Friday, Sunday",IF($C28="Prosperity","Monday, Thursday, Sunday",IF($C28="Diligence","Tuesday, Friday, Sunday",IF($C28="Gold","Wednesday, Saturday, Sunday"))))))</f>
+        <v>Wednesday, Saturday, Sunday</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G28" s="1" t="str">
+        <f t="shared" ref="G28:G34" si="3">IF($B28="Geo","Prithiva Topaz (Geo Hypostasis)",IF($B28="Pyro","Agnidus Agate (Pyro Regisvine)",IF($B28="Hydro","Varunada Lazurite (Oceanid)",IF($B28="Electro","Vajrada Amethyst (Electro Hypostasis)",IF($B28="Cryo","Shivada Jade (Cryo Regisvine)",IF($B28="Anemo","Vayuda Turquoise (Anemo Hypostasis)"))))))</f>
+        <v>Vayuda Turquoise (Anemo Hypostasis)</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="1" t="str">
+      <c r="D29" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Tuesday, Friday, Sunday</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="G29" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Agnidus Agate (Pyro Regisvine)</v>
       </c>
-      <c r="H28" s="1" t="s">
+      <c r="H29" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="5" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C30" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D29" s="1" t="str">
+      <c r="D30" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Monday, Thursday, Sunday</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="G29" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="G30" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Vayuda Turquoise (Anemo Hypostasis)</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H30" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="I29" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v>Wednesday, Saturday, Sunday</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G30" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Varunada Lazurite (Oceanid)</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="I30" s="1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>42</v>
@@ -1991,27 +2001,27 @@
         <v>Wednesday, Saturday, Sunday</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G31" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>Agnidus Agate (Pyro Regisvine)</v>
+        <f t="shared" si="3"/>
+        <v>Varunada Lazurite (Oceanid)</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="A32" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -2021,29 +2031,29 @@
         <f t="shared" si="2"/>
         <v>Wednesday, Saturday, Sunday</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>86</v>
+      <c r="E32" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="G32" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>Agnidus Agate (Pyro Regisvine)</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>28</v>
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>42</v>
@@ -2052,31 +2062,62 @@
         <f t="shared" si="2"/>
         <v>Wednesday, Saturday, Sunday</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E33" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>Agnidus Agate (Pyro Regisvine)</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>Wednesday, Saturday, Sunday</v>
+      </c>
+      <c r="E34" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F33" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G33" s="1" t="str">
-        <f t="shared" si="1"/>
+      <c r="G34" s="1" t="str">
+        <f t="shared" si="3"/>
         <v>Prithiva Topaz (Geo Hypostasis)</v>
       </c>
-      <c r="H33" s="1" t="s">
+      <c r="H34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="I33" s="1" t="s">
+      <c r="I34" s="1" t="s">
         <v>112</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E9" r:id="rId1" xr:uid="{E9838062-4EDF-40DB-A630-5CAF90CDC032}"/>
-    <hyperlink ref="E12" r:id="rId2" xr:uid="{6513F672-D58A-4418-88DF-CD88FCFE21D2}"/>
-    <hyperlink ref="E14" r:id="rId3" xr:uid="{5DE0E8BA-5E16-41A3-9A96-306289C2D9FA}"/>
-    <hyperlink ref="E17" r:id="rId4" xr:uid="{3C058029-A86C-4878-BFA2-F953AB959878}"/>
-    <hyperlink ref="E20" r:id="rId5" xr:uid="{73DB4A3D-39F5-4BFA-BEF8-DFD4DE41F1C6}"/>
-    <hyperlink ref="E32" r:id="rId6" xr:uid="{FDE45708-3BED-4F0B-914A-25739BDEE298}"/>
+    <hyperlink ref="E13" r:id="rId2" xr:uid="{6513F672-D58A-4418-88DF-CD88FCFE21D2}"/>
+    <hyperlink ref="E15" r:id="rId3" xr:uid="{5DE0E8BA-5E16-41A3-9A96-306289C2D9FA}"/>
+    <hyperlink ref="E18" r:id="rId4" xr:uid="{3C058029-A86C-4878-BFA2-F953AB959878}"/>
+    <hyperlink ref="E21" r:id="rId5" xr:uid="{73DB4A3D-39F5-4BFA-BEF8-DFD4DE41F1C6}"/>
+    <hyperlink ref="E33" r:id="rId6" xr:uid="{FDE45708-3BED-4F0B-914A-25739BDEE298}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>

</xml_diff>